<commit_message>
add interceptor handle error
</commit_message>
<xml_diff>
--- a/document/Project Structure.xlsx
+++ b/document/Project Structure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F50CF10B-7A70-46D2-B437-AD5049E62932}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29C22BB7-7300-4AC0-8B65-EE1653F77736}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Request</t>
   </si>
@@ -84,6 +84,12 @@
   <si>
     <t>Create Util common: DateUtil, StringUtil, CollectionUtil…</t>
   </si>
+  <si>
+    <t>19/8/2018</t>
+  </si>
+  <si>
+    <t>13/8/2018</t>
+  </si>
 </sst>
 </file>
 
@@ -141,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -170,6 +176,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -206,8 +215,8 @@
       <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>70</xdr:col>
-      <xdr:colOff>145675</xdr:colOff>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
@@ -225,9 +234,9 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="3735482" y="392206"/>
-          <a:ext cx="11745443" cy="6650692"/>
+          <a:ext cx="10580592" cy="6650692"/>
           <a:chOff x="3821207" y="974912"/>
-          <a:chExt cx="12012703" cy="6645089"/>
+          <a:chExt cx="10821347" cy="6645089"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -822,8 +831,8 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="12774706" y="773206"/>
-                <a:ext cx="1120589" cy="481852"/>
+                <a:off x="12774705" y="773206"/>
+                <a:ext cx="1120589" cy="331423"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -914,8 +923,8 @@
             </xdr:nvCxnSpPr>
             <xdr:spPr>
               <a:xfrm rot="10800000" flipV="1">
-                <a:off x="10247782" y="1014131"/>
-                <a:ext cx="2526925" cy="252133"/>
+                <a:off x="10247782" y="938917"/>
+                <a:ext cx="2526924" cy="327347"/>
               </a:xfrm>
               <a:prstGeom prst="bentConnector2">
                 <a:avLst/>
@@ -1506,8 +1515,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="13884087" y="974912"/>
-            <a:ext cx="1949823" cy="3339352"/>
+            <a:off x="13884086" y="974912"/>
+            <a:ext cx="758468" cy="3433949"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1538,7 +1547,7 @@
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="l"/>
@@ -2129,6 +2138,137 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541D5FB8-561F-463B-906A-646C4855C5E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8905875" y="4743450"/>
+          <a:ext cx="1066800" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Metadata</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>188359</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="TextBox 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAF5FB4-9C9B-440F-8238-28DC49210644}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6048375" y="5476876"/>
+          <a:ext cx="931309" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Metadata</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2531,8 +2671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935BE1C8-1993-4484-AE4B-D5636BDBFC0A}">
   <dimension ref="N6:AS17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BE25" sqref="BE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,8 +2704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,7 +2759,12 @@
         <v>13</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -2629,8 +2774,12 @@
         <v>14</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -2640,7 +2789,12 @@
         <v>15</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -2650,7 +2804,12 @@
         <v>16</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">

</xml_diff>